<commit_message>
updated beer tables to include manf price
</commit_message>
<xml_diff>
--- a/code/table_generation/beers_table.xlsx
+++ b/code/table_generation/beers_table.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="122">
   <si>
     <t>id</t>
   </si>
@@ -38,9 +38,6 @@
     <t>manf</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>manf_price</t>
   </si>
   <si>
@@ -89,21 +86,9 @@
     <t>Bud Light Platinum</t>
   </si>
   <si>
-    <t>lager</t>
-  </si>
-  <si>
-    <t>light beer</t>
-  </si>
-  <si>
-    <t>amber lager</t>
-  </si>
-  <si>
     <t>Rolling Rock</t>
   </si>
   <si>
-    <t>pale lager</t>
-  </si>
-  <si>
     <t>Busch</t>
   </si>
   <si>
@@ -113,15 +98,9 @@
     <t>Busch Ice</t>
   </si>
   <si>
-    <t>ice beer</t>
-  </si>
-  <si>
     <t>Shock Top</t>
   </si>
   <si>
-    <t>Belgian-style wheat ale</t>
-  </si>
-  <si>
     <t>Natural Light</t>
   </si>
   <si>
@@ -132,9 +111,6 @@
   </si>
   <si>
     <t>Coors Light</t>
-  </si>
-  <si>
-    <t>dark lager</t>
   </si>
   <si>
     <t>Keystone</t>
@@ -423,6 +399,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="174" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -452,8 +431,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E94" sqref="E94"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -747,7 +727,7 @@
     <col min="6" max="6" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -758,1464 +738,1810 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
       <c r="D2">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E2" s="1">
+        <f ca="1">NORMINV(RAND(),0.6,0.1)</f>
+        <v>0.73401696421275209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>4.2</v>
       </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E26" ca="1" si="0">NORMINV(RAND(),0.6,0.1)</f>
+        <v>0.60732800020543842</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>6</v>
       </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.64985995847143219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>5.0999999999999996</v>
       </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.63779636911882054</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.66329669940924929</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.64039284174605138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.704841653535487</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <v>4.5</v>
       </c>
-      <c r="F9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E9" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.72988789122997344</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10">
         <v>4.3</v>
       </c>
-      <c r="F10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E10" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.56328108310351677</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11">
         <v>4.0999999999999996</v>
       </c>
-      <c r="F11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E11" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.57188488788082714</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12">
         <v>5.9</v>
       </c>
-      <c r="F12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E12" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.47604023687332581</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13">
         <v>5.2</v>
       </c>
-      <c r="F13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E13" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.48458268262232634</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D14">
         <v>4.2</v>
       </c>
-      <c r="F14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E14" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.63357284433565564</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15">
         <v>5.9</v>
       </c>
-      <c r="F15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E15" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.69914079765120352</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D16">
         <v>4.5999999999999996</v>
       </c>
-      <c r="F16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E16" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.76209100957143749</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D17">
         <v>5.4</v>
       </c>
-      <c r="F17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E17" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.45774450567214625</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18">
         <v>5</v>
       </c>
-      <c r="F18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E18" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.85568429882879027</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19">
         <v>4.9000000000000004</v>
       </c>
-      <c r="F19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E19" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.48688849236850518</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E20" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.69114486632826755</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E21" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.71305259189198078</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D22">
         <v>5</v>
       </c>
-      <c r="F22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E22" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.5363898146785957</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D23">
         <v>4.2</v>
       </c>
-      <c r="F23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E23" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.65634407926252702</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D24">
         <v>4.8</v>
       </c>
-      <c r="F24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E24" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.69804344377560879</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D25">
         <v>4.2</v>
       </c>
-      <c r="F25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E25" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.61259021072796738</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D26">
         <v>5.9</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E26" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.62254557036138625</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D27">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E27" s="1">
+        <f ca="1">NORMINV(RAND(),0.75,0.15)</f>
+        <v>0.68919171051367256</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D28">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E28" s="1">
+        <f t="shared" ref="E28:E37" ca="1" si="1">NORMINV(RAND(),0.75,0.15)</f>
+        <v>0.65920639936527792</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D29">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E29" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.7648551061144071</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D30">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E30" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.5547660368734354</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C31" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D31">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E31" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.89501384384401228</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C32" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D32">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.84127370147895009</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C33" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D33">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.58040470872685246</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C34" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D34">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.79145105070740007</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C35" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D35">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.59245931043966737</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D36">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.75376529292859495</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C37" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D37">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.53580857925753</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C38" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D38">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38" s="1">
+        <f ca="1">NORMINV(RAND(),0.6,0.1)</f>
+        <v>0.6761336781946119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C39" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D39">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39" s="1">
+        <f t="shared" ref="E39:E45" ca="1" si="2">NORMINV(RAND(),0.6,0.1)</f>
+        <v>0.43456940491063029</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C40" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D40">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.53393766198741532</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C41" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D41">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.57274631321654335</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C42" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D42">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.78057011906388585</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C43" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D43">
         <v>8.1</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.70304486352115547</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C44" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D44">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.60593184113772269</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C45" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D45">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.71326398483364184</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C46" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D46">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46" s="1">
+        <f ca="1">NORMINV(RAND(),0.75,0.15)</f>
+        <v>0.82142861482294205</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C47" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D47">
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47" s="1">
+        <f t="shared" ref="E47:E49" ca="1" si="3">NORMINV(RAND(),0.75,0.15)</f>
+        <v>1.1142756363340824</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C48" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D48">
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.79730820342051578</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C49" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D49">
         <v>8</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.52014464549648798</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C50" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D50">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50" s="1">
+        <f ca="1">NORMINV(RAND(),0.85,0.15)</f>
+        <v>0.82525230966435426</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C51" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D51">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51" s="1">
+        <f t="shared" ref="E51:E56" ca="1" si="4">NORMINV(RAND(),0.85,0.15)</f>
+        <v>0.85991232474162715</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C52" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D52">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.62390667599351868</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C53" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D53">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.86313596009165949</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C54" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D54">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.94438150891219896</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C55" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D55">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.82374610493811051</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C56" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D56">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.65473892794585742</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C57" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D57">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57" s="1">
+        <f ca="1">NORMINV(RAND(),0.85,0.15)</f>
+        <v>0.62030783551345992</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C58" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D58">
         <v>5.2</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58" s="1">
+        <f ca="1">NORMINV(RAND(),1,0.2)</f>
+        <v>0.92187684871987385</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C59" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D59">
         <v>5.9</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59" s="1">
+        <f t="shared" ref="E59:E68" ca="1" si="5">NORMINV(RAND(),1,0.2)</f>
+        <v>0.75096704262779801</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C60" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D60">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.84584777927716182</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C61" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D61">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.86777696203883348</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C62" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D62">
         <v>6.9</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>1.2561111267224843</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C63" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D63">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>1.0900564895931772</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C64" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D64">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.86761976444394273</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C65" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D65">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>1.2123376695177515</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C66" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D66">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>1.1047864505929303</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C67" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D67">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>1.0211345837879366</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C68" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D68">
         <v>5</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.93403963744019791</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C69" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D69">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69" s="1">
+        <f ca="1">NORMINV(RAND(),1.1,0.2)</f>
+        <v>1.4253993307280699</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C70" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D70">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70" s="1">
+        <f t="shared" ref="E70:E85" ca="1" si="6">NORMINV(RAND(),1.1,0.2)</f>
+        <v>0.79156344853042804</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C71" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D71">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.94723179451201145</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C72" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D72">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>1.0473964821805977</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C73" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D73">
         <v>5.2</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.72880116863255817</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C74" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D74">
         <v>6</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.7540293400397704</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C75" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D75">
         <v>7</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>1.2263730737952745</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C76" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D76">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.97661945297821884</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C77" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D77">
         <v>5.2</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.75376714220638197</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C78" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D78">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E78" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.72969298187685805</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C79" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D79">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E79" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>1.4000582123689536</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C80" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D80">
         <v>5</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E80" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>1.492526107359752</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C81" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D81">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E81" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.97484255739831061</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C82" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D82">
         <v>6</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E82" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>1.2117347743882314</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C83" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D83">
         <v>17.5</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E83" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>1.1637385476222837</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C84" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D84">
         <v>6</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E84" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>1.0671046549462058</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C85" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D85">
         <v>9</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E85" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>1.1003725875548844</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C86" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D86">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E86" s="1">
+        <f ca="1">NORMINV(RAND(),0.85,0.15)</f>
+        <v>0.59872288256675865</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C87" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D87">
         <v>5</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E87" s="1">
+        <f t="shared" ref="E87:E90" ca="1" si="7">NORMINV(RAND(),0.85,0.15)</f>
+        <v>1.2189864559288435</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C88" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D88">
         <v>5.8</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E88" s="1">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.90531497959854623</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C89" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D89">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E89" s="1">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.95110782185906872</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C90" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D90">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E90" s="1">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.872343469307304</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C91" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D91">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E91" s="1">
+        <f ca="1">NORMINV(RAND(),0.6,0.1)</f>
+        <v>0.64524227794330324</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C92" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D92">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E92" s="1">
+        <f t="shared" ref="E92:E98" ca="1" si="8">NORMINV(RAND(),0.6,0.1)</f>
+        <v>0.43563239845624596</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C93" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D93">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E93" s="1">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.74786587520285219</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C94" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D94">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E94" s="1">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.52786938311497855</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C95" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D95">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E95" s="1">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.56634654020964426</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C96" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D96">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E96" s="1">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.63995151739868139</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C97" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D97">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E97" s="1">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.64285500639971782</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C98" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D98">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E98" s="1">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.64739805976437881</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C99" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="D99">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E99" s="1">
+        <f ca="1">NORMINV(RAND(),1.1,0.2)</f>
+        <v>0.88267006567963235</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>127</v>
+        <v>119</v>
+      </c>
+      <c r="C100" t="s">
+        <v>118</v>
       </c>
       <c r="D100">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E100" s="1">
+        <f t="shared" ref="E100:E101" ca="1" si="9">NORMINV(RAND(),1.1,0.2)</f>
+        <v>1.2267277038953153</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>128</v>
+        <v>120</v>
+      </c>
+      <c r="C101" t="s">
+        <v>118</v>
       </c>
       <c r="D101">
         <v>5.8</v>
+      </c>
+      <c r="E101" s="1">
+        <f t="shared" ca="1" si="9"/>
+        <v>1.2381788747139577</v>
       </c>
     </row>
   </sheetData>

</xml_diff>